<commit_message>
Benchmarked 2nd batch of web search logs obtained with 'openai' mode
</commit_message>
<xml_diff>
--- a/benchmark_logs/2nd-benchmark-session/benchmark-milestones.xlsx
+++ b/benchmark_logs/2nd-benchmark-session/benchmark-milestones.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI17"/>
+  <dimension ref="A1:BI19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -918,7 +918,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>cve_id_exists</t>
+          <t>cve_id_ok</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1225,7 +1225,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>main_service_identified</t>
+          <t>main_service</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>main_service_version</t>
+          <t>main_version</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1839,7 +1839,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>aux_roles_ok</t>
+          <t>aux_services</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2146,7 +2146,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>services_implemented_in_code</t>
+          <t>docker_runs</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2181,17 +2181,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -2211,17 +2211,17 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -2241,52 +2241,52 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AH8" t="inlineStr">
@@ -2316,27 +2316,27 @@
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
@@ -2351,17 +2351,17 @@
       </c>
       <c r="AP8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AR8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AS8" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="AU8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AV8" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="AW8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AX8" t="inlineStr">
@@ -2396,64 +2396,64 @@
       </c>
       <c r="AY8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AZ8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BA8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BB8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BC8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BD8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BE8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BF8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BG8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BH8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BI8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>main_service_uses_vulnerable_version</t>
+          <t>services_ok</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -2518,12 +2518,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -2553,47 +2553,47 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AH9" t="inlineStr">
@@ -2628,12 +2628,12 @@
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="AP9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AQ9" t="inlineStr">
@@ -2708,42 +2708,42 @@
       </c>
       <c r="AZ9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BA9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BB9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BC9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BD9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BE9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BF9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BG9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BH9" t="inlineStr">
@@ -2753,14 +2753,14 @@
       </c>
       <c r="BI9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>docker_runs</t>
+          <t>code_main_version</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2795,17 +2795,17 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2825,17 +2825,17 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -2860,12 +2860,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -2880,12 +2880,12 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
@@ -2895,12 +2895,12 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="AG10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AH10" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="AU10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AV10" t="inlineStr">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="AW10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AX10" t="inlineStr">
@@ -3020,37 +3020,37 @@
       </c>
       <c r="BA10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BB10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BC10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BD10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BE10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BF10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BG10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BH10" t="inlineStr">
@@ -3060,14 +3060,14 @@
       </c>
       <c r="BI10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>docker_vulnerable_to_cve</t>
+          <t>docker_vulnerable</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3132,12 +3132,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="AP11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AQ11" t="inlineStr">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="AR11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AS11" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="BG11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BH11" t="inlineStr">
@@ -3367,14 +3367,14 @@
       </c>
       <c r="BI11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>exploit_returns_expected_result</t>
+          <t>exploitable</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4651,6 +4651,380 @@
       </c>
       <c r="BI17" t="n">
         <v>0.02698</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Test Iterations</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>10</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>10</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" t="n">
+        <v>10</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>10</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>10</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>3</v>
+      </c>
+      <c r="V18" t="n">
+        <v>3</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>3</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Number of Containers</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>2</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>3</v>
+      </c>
+      <c r="U19" t="n">
+        <v>4</v>
+      </c>
+      <c r="V19" t="n">
+        <v>4</v>
+      </c>
+      <c r="W19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>